<commit_message>
Data - se actualiza los xml con la infoprmacion dada y se crean los json en public
</commit_message>
<xml_diff>
--- a/updateINFO/data/projectsMBE.xlsx
+++ b/updateINFO/data/projectsMBE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="106">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">fundingAgency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">socialNetwork_fb</t>
   </si>
   <si>
     <t xml:space="preserve">socialNetwork_x</t>
@@ -252,6 +255,134 @@
   <si>
     <t xml:space="preserve">CHALLENGE2_MICINN</t>
   </si>
+  <si>
+    <t xml:space="preserve">carreras@ub.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos Carreras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIFE TURTLENEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caretta caretta nesting range expansion under climate warming: urgent actions to mitigate threats at emerging nesting sites in the Western Mediterranean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIFE21-NAT-IT-LIFE-TURTLENEST/101074584 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">09-01-2028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08-4-2028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loggerhead turtles are expanding their nesting range into the western Mediterranean, where beaches are becoming suitable because of climate warming. However, emerging nesting sites are threatened by coastal development and high tourist pressure (light pollution, recreational activities and beach management practices). In the eastern Mediterranean, where the vast majority of loggerhead turtle nesting occurs, conservation projects over the past 30 years have helped mitigate these threats and accustomed tourists and other stakeholders to the presence and needs of sea turtles during the nesting season. This has not happened in the western Mediterranean as colonisation by nesting loggerhead turtles is ongoing; people on the beaches in this region are often unprepared because of a general lack of awareness and knowledge of this range expasion. For more than a decade, nesting remained occasional, with only 13 loggerhead turtle nests recorded in the entire western Mediterranean up to 2012. However, since 2013 the number of nests in this region has increased rapidly, with record numbers of 79 in 2020 and 100 in 2021. This increased nesting activity is considered to be an adaptive response to changing environmental conditions due to climate warming and the consequent opening up of new sites suitable for nesting. However, beaches in the western Mediterranean have long been exploited by humans and few pristine places suitable for loggerhead turtle nesting remain. LIFE TURTLENEST aims to mitigate threats to the species in Italy, Spain and France in order to protect new nesting habitats and foster successful sea turtle reproduction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.legambiente.it/progetti/lifeturtlenest/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programme for Environment and Climate Action (LIFE).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.facebook.com/profile.php?id=100091570414407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://x.com/LifeTurtlenest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.instagram.com/life_turtlenest/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logo_turtlenest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fundingLIFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TortugaCarlos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos Carreras &amp; Owen S. Wangensteen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlueDNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conservation and management of keystone marine species, from genomes to populations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PID2023-146307OB-C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-09-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08-31-2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The development and application of high throughput techniques (HTS) has revolutionized the field of conservation genomics and has provided novel tools to answer relevant scientific questions for the management and conservation of keystone species. The assembly and annotation of quality reference genomes is a centerpiece of this discipline. However, a single reference genome is unable to capture all species diversity. Our results from the previous projects demonstrate that building a pangenome by combining a reference genome with whole genome sequences across the species distribution is key to unveil the genome complexity across populations. The subproject BlueDNA-I will follow this approach to resolve detected research challenges on key marine species. We will first annotate quality reference genomes from parallel projects and build pangenomes using whole genome sequencing on individuals across the species Distribution area. This information will be combined with fine-scale population genomics data to address connectivity and adaptation. As a summary, BlueDNA-I aims to do a step forward on the application of genomics, particularly by building pangenomes, on key species for management and conservation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCIN/ AEI/10.13039/501100011033 and ERDF/EU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fundingBLUEDNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlueDNACarlos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InGeNi-Caretta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigación para la gestión y protección de la nidificación de tortugas marinas: colonización de la tortuga careta (Caretta caretta) en el Mediterráneo occidental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-05-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-31-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Mediterráneo occidental está experimentando un incremento de la nidificación de la tortuga careta o tortuga boba (Caretta caretta) que se corresponde con un proceso de colonización de la especie como respuesta al cambio climático. Este fenómeno se considera de gran importancia para su supervivencia debido a las predicciones de
+feminización y reducción de la viabilidad de crías en las playas de puesta de origen mientras que las nuevas playas de puesta presentan condiciones más favorables en un escenario de calentamiento global. Sin embargo, esta colonización se produce en una zona con una elevada ocupación humana, como el litoral español, por lo que es necesaria una gestión adecuada para favorecer el éxito de estas puestas en convivencia con la presencia humana. Por desgracia, la gestión de este fenómeno de colonización se ve comprometida por una escasez de información científica sobre la creciente población, la idoneidad de las playas de puesta y la efectividad de las medidas de gestión que se están implementando.
+En este contexto, InGeNi-Caretta es un proyecto multidisciplinar con un equipo investigador compuesto por destacados expertos en tortugas marinas con la finalidad de generar los conocimientos científicos necesarios para facilitar la toma de decisiones en la planificación y gestión de esta especie amenazada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biodiversity Foundation of the Ministry for the Ecological Transition and the Demographic Challenge (MITECO) of the Government of Spain, within the framework of the Recovery, Transformation and Resilience Plan (PRTR), funded by the European Union - NextGenerationEU.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fundingInGeNi-Caretta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hatchzoomCarlos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GenoMarTur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genome diversity for marine turtle management and conservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNS2022-135205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-09-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marine turtles are iconic species of conservation concern and focalised research is needed to aid their management and conservation. Genetic approaches have been extensively used due to the highly migratory behaviour of marine turtles and because they spend most of their lives at sea. Their philopatric behaviour produces deep population genetic structuring, and thus genetic approaches are needed to delineate management and conservation units. Furthermore, their long migrations in time and space demand tools to assess the origin of the individuals found at sea to be able to link threats in foraging areas to the nesting populations affected. However, these studies have been hampered by the limited resolution of the genetic approaches used and, for this reason, the development of new genomic tools is needed to improve the results and also allow to explore new relevant research features, such as the detection of genomic signals of adaptation. One of the last improvements in marine turtle genomics has been the development of chromosome level reference genomes for the loggerhead (Caretta caretta) the green (Chelonia mydas) and the leatherback (Dermochelys coriacea) marine turtles. However, a single reference genome is not enough to capture the species-specific diversity in terms of structural and sequence variants. The project GenoMarTur aims to characterise the genome diversity of these three species and use this valuable information to resolve key questions on marine turtle research aiming to improve their management and conservation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MICIU/AEI/10.13039/501100011033/ and by the “European Union NextGenerationEU/PRTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fundingGenomediversity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TortugaManu</t>
+  </si>
 </sst>
 </file>
 
@@ -260,7 +391,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -288,7 +419,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -296,7 +427,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -330,21 +461,56 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color rgb="FF434343"/>
       <name val="Roboto"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF434343"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFF8F9FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -532,8 +698,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -557,8 +824,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -611,6 +881,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -635,11 +909,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -671,16 +949,77 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -692,6 +1031,38 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF434343"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F9FA"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF1155CC"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -721,7 +1092,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -729,7 +1100,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF1155CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -753,7 +1124,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF5B3F86"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -761,16 +1132,16 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF5B3F86"/>
       <rgbColor rgb="FF442F65"/>
+      <rgbColor rgb="FF434343"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:P5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:Q9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="17">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="email"/>
     <tableColumn id="3" name="researcher"/>
@@ -783,10 +1154,11 @@
     <tableColumn id="10" name="summary"/>
     <tableColumn id="11" name="websiteProject"/>
     <tableColumn id="12" name="fundingAgency"/>
-    <tableColumn id="13" name="socialNetwork_x"/>
-    <tableColumn id="14" name="socialNetwork_bsky"/>
-    <tableColumn id="15" name="socialNetwork_inst"/>
-    <tableColumn id="16" name="imageID_logo"/>
+    <tableColumn id="13" name="socialNetwork_fb"/>
+    <tableColumn id="14" name="socialNetwork_x"/>
+    <tableColumn id="15" name="socialNetwork_bsky"/>
+    <tableColumn id="16" name="socialNetwork_inst"/>
+    <tableColumn id="17" name="imageID_logo"/>
   </tableColumns>
 </table>
 </file>
@@ -968,31 +1340,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="R9" activeCellId="0" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="37.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="132.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="22.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="33.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="27.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="25.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="18" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="37.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="18.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="132.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="25.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="18.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="19" style="1" width="18.86"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,7 +1413,7 @@
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="6" t="s">
@@ -1056,219 +1428,404 @@
       <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="0"/>
-      <c r="X1" s="0"/>
-      <c r="Y1" s="0"/>
-      <c r="Z1" s="0"/>
+      <c r="U1" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" s="12" customFormat="true" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="12" customFormat="true" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" s="12" customFormat="true" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="C3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="8" t="s">
+      <c r="D3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="12" t="s">
+      <c r="L3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="N3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="0"/>
-      <c r="X2" s="0"/>
-      <c r="Y2" s="0"/>
-      <c r="Z2" s="0"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="22"/>
+      <c r="S3" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="3" s="12" customFormat="true" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="W3" s="0"/>
-      <c r="X3" s="0"/>
-      <c r="Y3" s="0"/>
-      <c r="Z3" s="0"/>
-    </row>
-    <row r="4" s="12" customFormat="true" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" s="12" customFormat="true" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>42</v>
+        <v>22</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="H4" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="M4" s="13"/>
+      <c r="N4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="W4" s="0"/>
-      <c r="X4" s="0"/>
-      <c r="Y4" s="0"/>
-      <c r="Z4" s="0"/>
+      <c r="S4" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" s="12" customFormat="true" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="n">
+    <row r="5" s="12" customFormat="true" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="D5" s="26" t="s">
         <v>53</v>
       </c>
+      <c r="E5" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="F5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="H5" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="I5" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="J5" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="K5" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="12" t="s">
+      <c r="L5" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="M5" s="13"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="W5" s="0"/>
-      <c r="X5" s="0"/>
-      <c r="Y5" s="0"/>
-      <c r="Z5" s="0"/>
+      <c r="R5" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="30" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" s="30"/>
+      <c r="P6" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q6" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="S6" s="39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="42"/>
+      <c r="R7" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="S7" s="39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="M8" s="42"/>
+      <c r="R8" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="S8" s="39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="M9" s="42"/>
+      <c r="R9" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="S9" s="39" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K6" r:id="rId1" display="https://www.legambiente.it/progetti/lifeturtlenest/"/>
+    <hyperlink ref="M6" r:id="rId2" display="https://www.facebook.com/profile.php?id=100091570414407"/>
+    <hyperlink ref="N6" r:id="rId3" display="https://x.com/LifeTurtlenest"/>
+    <hyperlink ref="P6" r:id="rId4" display="https://www.instagram.com/life_turtlenest/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1277,7 +1834,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se aplican los comentrios del correo del 20-jun-2025, 12 puntos anotados en bitacora
</commit_message>
<xml_diff>
--- a/updateINFO/data/projectsMBE.xlsx
+++ b/updateINFO/data/projectsMBE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -138,7 +138,7 @@
     <t xml:space="preserve">https://x.com/EchinoAdaptive</t>
   </si>
   <si>
-    <t xml:space="preserve">logo_enviome2</t>
+    <t xml:space="preserve">logo_enviome</t>
   </si>
   <si>
     <t xml:space="preserve">ACIDOMIC</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">MCIN and the European Union NextGeneration</t>
   </si>
   <si>
-    <t xml:space="preserve">logo_acidomic2</t>
+    <t xml:space="preserve">logo_acidomic</t>
   </si>
   <si>
     <t xml:space="preserve">paracentrotus_Rocío</t>
@@ -207,7 +207,7 @@
     <t xml:space="preserve">Fundación BBVA</t>
   </si>
   <si>
-    <t xml:space="preserve">logo_divergen2</t>
+    <t xml:space="preserve">logo_divergen</t>
   </si>
   <si>
     <t xml:space="preserve">divergen_team</t>
@@ -244,16 +244,13 @@
 relevance for our planet. The integration of all the results generated (human pressures and natural hazards) that currently challenge the Antarctic marine ecosystems, together with previous general knowledge for the Antarctic Peninsula and nearby areas will produce a huge dataset of useful information for other researchers and for better managing these endangered habitats.</t>
   </si>
   <si>
-    <t xml:space="preserve">none</t>
-  </si>
-  <si>
     <t xml:space="preserve">MICINN</t>
   </si>
   <si>
-    <t xml:space="preserve">logo_CHALLENGE2_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHALLENGE2_MICINN</t>
+    <t xml:space="preserve">logo_CHALLENGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHALLENGE_MICINN</t>
   </si>
   <si>
     <t xml:space="preserve">carreras@ub.edu</t>
@@ -1342,10 +1339,10 @@
   </sheetPr>
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="R9" activeCellId="0" sqref="R9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1611,20 +1608,18 @@
       <c r="J5" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="25"/>
+      <c r="L5" s="25" t="s">
         <v>60</v>
-      </c>
-      <c r="L5" s="25" t="s">
-        <v>61</v>
       </c>
       <c r="M5" s="13"/>
       <c r="O5" s="29"/>
       <c r="P5" s="29"/>
       <c r="Q5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" s="22" t="s">
         <v>62</v>
-      </c>
-      <c r="R5" s="22" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,56 +1627,56 @@
         <v>5</v>
       </c>
       <c r="B6" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="D6" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="33" t="s">
+      <c r="F6" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="G6" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="H6" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="I6" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="J6" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="K6" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="L6" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="36" t="s">
+      <c r="M6" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="M6" s="37" t="s">
+      <c r="N6" s="37" t="s">
         <v>74</v>
-      </c>
-      <c r="N6" s="37" t="s">
-        <v>75</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="Q6" s="38" t="s">
+      <c r="R6" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="R6" s="39" t="s">
+      <c r="S6" s="39" t="s">
         <v>78</v>
-      </c>
-      <c r="S6" s="39" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,44 +1684,42 @@
         <v>6</v>
       </c>
       <c r="B7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="32" t="s">
-        <v>65</v>
-      </c>
       <c r="D7" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="F7" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="H7" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="I7" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="J7" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="K7" s="25"/>
+      <c r="L7" s="41" t="s">
         <v>86</v>
-      </c>
-      <c r="K7" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" s="41" t="s">
-        <v>87</v>
       </c>
       <c r="M7" s="42"/>
       <c r="R7" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="S7" s="39" t="s">
         <v>88</v>
-      </c>
-      <c r="S7" s="39" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,44 +1727,42 @@
         <v>7</v>
       </c>
       <c r="B8" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="32" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="27" t="s">
+      <c r="I8" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="J8" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="J8" s="43" t="s">
+      <c r="K8" s="25"/>
+      <c r="L8" s="43" t="s">
         <v>94</v>
-      </c>
-      <c r="K8" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="L8" s="43" t="s">
-        <v>95</v>
       </c>
       <c r="M8" s="42"/>
       <c r="R8" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="S8" s="39" t="s">
         <v>96</v>
-      </c>
-      <c r="S8" s="39" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,44 +1770,42 @@
         <v>8</v>
       </c>
       <c r="B9" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="32" t="s">
-        <v>65</v>
-      </c>
       <c r="D9" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="H9" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="I9" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="I9" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" s="44" t="s">
+      <c r="K9" s="25"/>
+      <c r="L9" s="44" t="s">
         <v>102</v>
-      </c>
-      <c r="K9" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="L9" s="44" t="s">
-        <v>103</v>
       </c>
       <c r="M9" s="42"/>
       <c r="R9" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="S9" s="39" t="s">
         <v>104</v>
-      </c>
-      <c r="S9" s="39" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se incluye en el excell-projects  el nombre de las imagenes recientemente enviadas para los proyectos de carlos y se genera el archivo .json
</commit_message>
<xml_diff>
--- a/updateINFO/data/projectsMBE.xlsx
+++ b/updateINFO/data/projectsMBE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -325,6 +325,9 @@
     <t xml:space="preserve">MCIN/ AEI/10.13039/501100011033 and ERDF/EU</t>
   </si>
   <si>
+    <t xml:space="preserve">BlueDNA_logo</t>
+  </si>
+  <si>
     <t xml:space="preserve">fundingBLUEDNA</t>
   </si>
   <si>
@@ -349,6 +352,9 @@
   </si>
   <si>
     <t xml:space="preserve">Biodiversity Foundation of the Ministry for the Ecological Transition and the Demographic Challenge (MITECO) of the Government of Spain, within the framework of the Recovery, Transformation and Resilience Plan (PRTR), funded by the European Union - NextGenerationEU.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingenicareta</t>
   </si>
   <si>
     <t xml:space="preserve">fundingInGeNi-Caretta</t>
@@ -825,7 +831,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -996,6 +1002,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1340,9 +1350,9 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
+      <selection pane="bottomLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1715,11 +1725,14 @@
         <v>86</v>
       </c>
       <c r="M7" s="42"/>
+      <c r="Q7" s="43" t="s">
+        <v>87</v>
+      </c>
       <c r="R7" s="39" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S7" s="39" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,33 +1749,36 @@
         <v>64</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="43" t="s">
-        <v>89</v>
-      </c>
       <c r="H8" s="27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="J8" s="43" t="s">
         <v>93</v>
       </c>
+      <c r="J8" s="44" t="s">
+        <v>94</v>
+      </c>
       <c r="K8" s="25"/>
-      <c r="L8" s="43" t="s">
-        <v>94</v>
+      <c r="L8" s="44" t="s">
+        <v>95</v>
       </c>
       <c r="M8" s="42"/>
+      <c r="Q8" s="43" t="s">
+        <v>96</v>
+      </c>
       <c r="R8" s="39" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="S8" s="39" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,33 +1795,33 @@
         <v>64</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>101</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="J9" s="44" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+      <c r="J9" s="45" t="s">
+        <v>103</v>
       </c>
       <c r="K9" s="25"/>
-      <c r="L9" s="44" t="s">
-        <v>102</v>
+      <c r="L9" s="45" t="s">
+        <v>104</v>
       </c>
       <c r="M9" s="42"/>
       <c r="R9" s="39" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="S9" s="39" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>